<commit_message>
🔄 Regenerate test files with corrected OFFSET test cases
- Regenerated Excel fixtures with corrected OFFSET error formulas
- Regenerated Python test classes with updated expectations
- All test files now reflect proper Excel behavior documentation
- Reduced test failures from 11 to 8 through proper test case validation

Co-authored-by: Ona <no-reply@ona.com>
</commit_message>
<xml_diff>
--- a/tests/resources/offset_errors.xlsx
+++ b/tests/resources/offset_errors.xlsx
@@ -617,13 +617,13 @@
     </row>
     <row r="3">
       <c r="F3">
-        <f>OFFSET(Data!A1, 100, 0)</f>
+        <f>OFFSET(Data!A1, 1048576, 0)</f>
         <v/>
       </c>
     </row>
     <row r="4">
       <c r="F4">
-        <f>OFFSET(Data!A1, 0, 100)</f>
+        <f>OFFSET(Data!A1, 0, 16384)</f>
         <v/>
       </c>
     </row>

</xml_diff>